<commit_message>
Works on Android 13
</commit_message>
<xml_diff>
--- a/Tests/AppAndroidUIAutomator2/AppAndroid.rvl.xlsx
+++ b/Tests/AppAndroidUIAutomator2/AppAndroid.rvl.xlsx
@@ -7,13 +7,14 @@
   </bookViews>
   <sheets>
     <sheet name="RVL" sheetId="1" r:id="rId2"/>
+    <sheet name="Debug" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="17">
   <si>
     <t>Flow</t>
   </si>
@@ -61,6 +62,9 @@
   </si>
   <si>
     <t>TestSiblings</t>
+  </si>
+  <si>
+    <t>DoDebug</t>
   </si>
 </sst>
 </file>
@@ -81,7 +85,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="161">
+  <borders count="323">
     <border>
       <left/>
       <right/>
@@ -249,11 +253,173 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="323">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -415,6 +581,168 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="158" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="159" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="160" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="161" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="162" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="163" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="164" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="165" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="166" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="167" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="168" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="169" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="170" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="171" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="172" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="173" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="174" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="175" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="176" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="177" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="178" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="179" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="180" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="181" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="182" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="183" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="184" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="185" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="186" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="187" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="188" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="189" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="190" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="191" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="192" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="193" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="194" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="195" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="196" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="197" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="198" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="199" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="200" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="201" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="202" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="203" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="204" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="205" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="206" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="207" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="208" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="209" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="210" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="211" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="212" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="214" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="215" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="216" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="218" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="219" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="220" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="222" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="223" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="224" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="226" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="227" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="228" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="229" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="230" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="231" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="232" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="234" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="235" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="236" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="237" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="238" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="239" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="240" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="241" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="242" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="243" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="244" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="245" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="246" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="247" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="248" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="249" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="250" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="251" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="252" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="254" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="255" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="256" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="257" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="258" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="259" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="260" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="261" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="262" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="263" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="264" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="265" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="266" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="267" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="268" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="269" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="270" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="271" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="272" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="273" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="274" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="275" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="276" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="277" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="278" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="279" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="280" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="281" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="282" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="283" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="284" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="285" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="286" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="287" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="288" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="289" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="290" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="291" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="292" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="293" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="294" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="295" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="296" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="297" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="298" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="299" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="300" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="301" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="302" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="303" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="304" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="305" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="306" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="307" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="308" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="309" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="310" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="311" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="312" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="313" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="314" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="315" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="316" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="317" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="318" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="319" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="320" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="322" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,16 +752,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H19"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.546875" customWidth="true"/>
     <col min="2" max="2" width="8.515625" customWidth="true"/>
-    <col min="3" max="3" width="12.49609375" customWidth="true"/>
-    <col min="4" max="4" width="12.49609375" customWidth="true"/>
-    <col min="5" max="5" width="12.49609375" customWidth="true"/>
-    <col min="6" max="6" width="12.49609375" customWidth="true"/>
-    <col min="7" max="7" width="12.49609375" customWidth="true"/>
+    <col min="3" max="3" width="12.4296875" customWidth="true"/>
+    <col min="4" max="4" width="12.4296875" customWidth="true"/>
+    <col min="5" max="5" width="12.4296875" customWidth="true"/>
+    <col min="6" max="6" width="12.4296875" customWidth="true"/>
+    <col min="7" max="7" width="12.4296875" customWidth="true"/>
     <col min="8" max="8" width="10.5390625" customWidth="true"/>
   </cols>
   <sheetData>
@@ -638,104 +966,341 @@
       <c r="H10" s="80"/>
     </row>
     <row r="11">
-      <c r="A11" s="81"/>
-      <c r="B11" s="82"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="85"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="87"/>
-      <c r="H11" s="88"/>
+      <c r="A11" s="89"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="95"/>
+      <c r="H11" s="96"/>
     </row>
     <row r="12">
-      <c r="A12" s="89"/>
-      <c r="B12" s="90"/>
-      <c r="C12" s="91"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="94"/>
-      <c r="G12" s="95"/>
-      <c r="H12" s="96"/>
+      <c r="A12" s="97"/>
+      <c r="B12" s="98"/>
+      <c r="C12" s="99"/>
+      <c r="D12" s="100"/>
+      <c r="E12" s="101"/>
+      <c r="F12" s="102"/>
+      <c r="G12" s="103"/>
+      <c r="H12" s="104"/>
     </row>
     <row r="13">
-      <c r="A13" s="97"/>
-      <c r="B13" s="98"/>
-      <c r="C13" s="99"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="103"/>
-      <c r="H13" s="104"/>
+      <c r="A13" s="105"/>
+      <c r="B13" s="106"/>
+      <c r="C13" s="107"/>
+      <c r="D13" s="108"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="110"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="112"/>
     </row>
     <row r="14">
-      <c r="A14" s="105"/>
-      <c r="B14" s="106"/>
-      <c r="C14" s="107"/>
-      <c r="D14" s="108"/>
-      <c r="E14" s="109"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="111"/>
-      <c r="H14" s="112"/>
+      <c r="A14" s="113"/>
+      <c r="B14" s="114"/>
+      <c r="C14" s="115"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="117"/>
+      <c r="F14" s="118"/>
+      <c r="G14" s="119"/>
+      <c r="H14" s="120"/>
     </row>
     <row r="15">
-      <c r="A15" s="113"/>
-      <c r="B15" s="114"/>
-      <c r="C15" s="115"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="117"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="119"/>
-      <c r="H15" s="120"/>
+      <c r="A15" s="121"/>
+      <c r="B15" s="122"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="124"/>
+      <c r="E15" s="125"/>
+      <c r="F15" s="126"/>
+      <c r="G15" s="127"/>
+      <c r="H15" s="128"/>
     </row>
     <row r="16">
-      <c r="A16" s="121"/>
-      <c r="B16" s="122"/>
-      <c r="C16" s="123"/>
-      <c r="D16" s="124"/>
-      <c r="E16" s="125"/>
-      <c r="F16" s="126"/>
-      <c r="G16" s="127"/>
-      <c r="H16" s="128"/>
+      <c r="A16" s="129"/>
+      <c r="B16" s="130"/>
+      <c r="C16" s="131"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="134"/>
+      <c r="G16" s="135"/>
+      <c r="H16" s="136"/>
     </row>
     <row r="17">
-      <c r="A17" s="129"/>
-      <c r="B17" s="130"/>
-      <c r="C17" s="131"/>
-      <c r="D17" s="132"/>
-      <c r="E17" s="133"/>
-      <c r="F17" s="134"/>
-      <c r="G17" s="135"/>
-      <c r="H17" s="136"/>
+      <c r="A17" s="137"/>
+      <c r="B17" s="138"/>
+      <c r="C17" s="139"/>
+      <c r="D17" s="140"/>
+      <c r="E17" s="141"/>
+      <c r="F17" s="142"/>
+      <c r="G17" s="143"/>
+      <c r="H17" s="144"/>
     </row>
     <row r="18">
-      <c r="A18" s="137"/>
-      <c r="B18" s="138"/>
-      <c r="C18" s="139"/>
-      <c r="D18" s="140"/>
-      <c r="E18" s="141"/>
-      <c r="F18" s="142"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="144"/>
+      <c r="A18" s="145"/>
+      <c r="B18" s="146"/>
+      <c r="C18" s="147"/>
+      <c r="D18" s="148"/>
+      <c r="E18" s="149"/>
+      <c r="F18" s="150"/>
+      <c r="G18" s="151"/>
+      <c r="H18" s="152"/>
     </row>
     <row r="19">
-      <c r="A19" s="145"/>
-      <c r="B19" s="146"/>
-      <c r="C19" s="147"/>
-      <c r="D19" s="148"/>
-      <c r="E19" s="149"/>
-      <c r="F19" s="150"/>
-      <c r="G19" s="151"/>
-      <c r="H19" s="152"/>
+      <c r="A19" s="153"/>
+      <c r="B19" s="154"/>
+      <c r="C19" s="155"/>
+      <c r="D19" s="156"/>
+      <c r="E19" s="157"/>
+      <c r="F19" s="158"/>
+      <c r="G19" s="159"/>
+      <c r="H19" s="160"/>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H21"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.546875" customWidth="true"/>
+    <col min="2" max="2" width="8.515625" customWidth="true"/>
+    <col min="3" max="3" width="12.4296875" customWidth="true"/>
+    <col min="4" max="4" width="12.4296875" customWidth="true"/>
+    <col min="5" max="5" width="12.4296875" customWidth="true"/>
+    <col min="6" max="6" width="12.4296875" customWidth="true"/>
+    <col min="7" max="7" width="12.4296875" customWidth="true"/>
+    <col min="8" max="8" width="10.5390625" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="161" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="162" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="163" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="164" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="165" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="166" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="167" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="168" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="169"/>
+      <c r="B2" s="170"/>
+      <c r="C2" s="171"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="173"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="176"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="321"/>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="177"/>
+      <c r="B4" s="178"/>
+      <c r="C4" s="179"/>
+      <c r="D4" s="180"/>
+      <c r="E4" s="181"/>
+      <c r="F4" s="182"/>
+      <c r="G4" s="183"/>
+      <c r="H4" s="184"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="185"/>
+      <c r="B5" s="186"/>
+      <c r="C5" s="187"/>
+      <c r="D5" s="188"/>
+      <c r="E5" s="189"/>
+      <c r="F5" s="190"/>
+      <c r="G5" s="191"/>
+      <c r="H5" s="192"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="193"/>
+      <c r="B6" s="194"/>
+      <c r="C6" s="195"/>
+      <c r="D6" s="196"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="198"/>
+      <c r="G6" s="199"/>
+      <c r="H6" s="200"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="201"/>
+      <c r="B7" s="202"/>
+      <c r="C7" s="203"/>
+      <c r="D7" s="204"/>
+      <c r="E7" s="205"/>
+      <c r="F7" s="206"/>
+      <c r="G7" s="207"/>
+      <c r="H7" s="208"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="209"/>
+      <c r="B8" s="210"/>
+      <c r="C8" s="211"/>
+      <c r="D8" s="212"/>
+      <c r="E8" s="213"/>
+      <c r="F8" s="214"/>
+      <c r="G8" s="215"/>
+      <c r="H8" s="216"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="217"/>
+      <c r="B9" s="218"/>
+      <c r="C9" s="219"/>
+      <c r="D9" s="220"/>
+      <c r="E9" s="221"/>
+      <c r="F9" s="222"/>
+      <c r="G9" s="223"/>
+      <c r="H9" s="224"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="225"/>
+      <c r="B10" s="226"/>
+      <c r="C10" s="227"/>
+      <c r="D10" s="228"/>
+      <c r="E10" s="229"/>
+      <c r="F10" s="230"/>
+      <c r="G10" s="231"/>
+      <c r="H10" s="232"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="233"/>
+      <c r="B11" s="234"/>
+      <c r="C11" s="235"/>
+      <c r="D11" s="236"/>
+      <c r="E11" s="237"/>
+      <c r="F11" s="238"/>
+      <c r="G11" s="239"/>
+      <c r="H11" s="240"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="241"/>
+      <c r="B12" s="242"/>
+      <c r="C12" s="243"/>
+      <c r="D12" s="244"/>
+      <c r="E12" s="245"/>
+      <c r="F12" s="246"/>
+      <c r="G12" s="247"/>
+      <c r="H12" s="248"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="249"/>
+      <c r="B13" s="250"/>
+      <c r="C13" s="251"/>
+      <c r="D13" s="252"/>
+      <c r="E13" s="253"/>
+      <c r="F13" s="254"/>
+      <c r="G13" s="255"/>
+      <c r="H13" s="256"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="257"/>
+      <c r="B14" s="258"/>
+      <c r="C14" s="259"/>
+      <c r="D14" s="260"/>
+      <c r="E14" s="261"/>
+      <c r="F14" s="262"/>
+      <c r="G14" s="263"/>
+      <c r="H14" s="264"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="265"/>
+      <c r="B15" s="266"/>
+      <c r="C15" s="267"/>
+      <c r="D15" s="268"/>
+      <c r="E15" s="269"/>
+      <c r="F15" s="270"/>
+      <c r="G15" s="271"/>
+      <c r="H15" s="272"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="273"/>
+      <c r="B16" s="274"/>
+      <c r="C16" s="275"/>
+      <c r="D16" s="276"/>
+      <c r="E16" s="277"/>
+      <c r="F16" s="278"/>
+      <c r="G16" s="279"/>
+      <c r="H16" s="280"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="281"/>
+      <c r="B17" s="282"/>
+      <c r="C17" s="283"/>
+      <c r="D17" s="284"/>
+      <c r="E17" s="285"/>
+      <c r="F17" s="286"/>
+      <c r="G17" s="287"/>
+      <c r="H17" s="288"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="289"/>
+      <c r="B18" s="290"/>
+      <c r="C18" s="291"/>
+      <c r="D18" s="292"/>
+      <c r="E18" s="293"/>
+      <c r="F18" s="294"/>
+      <c r="G18" s="295"/>
+      <c r="H18" s="296"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="297"/>
+      <c r="B19" s="298"/>
+      <c r="C19" s="299"/>
+      <c r="D19" s="300"/>
+      <c r="E19" s="301"/>
+      <c r="F19" s="302"/>
+      <c r="G19" s="303"/>
+      <c r="H19" s="304"/>
     </row>
     <row r="20">
-      <c r="A20" s="153"/>
-      <c r="B20" s="154"/>
-      <c r="C20" s="155"/>
-      <c r="D20" s="156"/>
-      <c r="E20" s="157"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="159"/>
-      <c r="H20" s="160"/>
+      <c r="A20" s="305"/>
+      <c r="B20" s="306"/>
+      <c r="C20" s="307"/>
+      <c r="D20" s="308"/>
+      <c r="E20" s="309"/>
+      <c r="F20" s="310"/>
+      <c r="G20" s="311"/>
+      <c r="H20" s="312"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="313"/>
+      <c r="B21" s="314"/>
+      <c r="C21" s="315"/>
+      <c r="D21" s="316"/>
+      <c r="E21" s="317"/>
+      <c r="F21" s="318"/>
+      <c r="G21" s="319"/>
+      <c r="H21" s="320"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>